<commit_message>
Ajustes:  - Se agrega atributo tipo_pot en la clase POT POT_FuenteAdministrativa  - Se agregan metadatos (escala, año y responsable) a la fuente espacial  - Se agregan soporte para geometrias tipo punto y linea a la clase POT_UE_SistemasGenerales  - Se actualiza el archivo de documentación de cambios propuestos
</commit_message>
<xml_diff>
--- a/DOCS/inventario_propuesta_ajustes_modelo.xlsx
+++ b/DOCS/inventario_propuesta_ajustes_modelo.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="91">
   <si>
     <t xml:space="preserve">SESION</t>
   </si>
@@ -312,7 +312,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -345,6 +345,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -404,13 +411,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD6DCE5"/>
-        <bgColor rgb="FFDEE6EF"/>
+        <bgColor rgb="FFE2F0D9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE2F0D9"/>
-        <bgColor rgb="FFDEE6EF"/>
+        <bgColor rgb="FFFBE5D6"/>
       </patternFill>
     </fill>
     <fill>
@@ -422,13 +429,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFFF"/>
-        <bgColor rgb="FFE2F0D9"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDEE6EF"/>
-        <bgColor rgb="FFD6DCE5"/>
+        <fgColor rgb="FF3465A4"/>
+        <bgColor rgb="FF44546A"/>
       </patternFill>
     </fill>
     <fill>
@@ -478,7 +485,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -567,6 +574,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -577,14 +588,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -616,37 +619,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDEE6EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3D3D3D"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -682,7 +654,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFDEE6EF"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFE2F0D9"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
@@ -695,7 +667,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFC55A11"/>
-      <rgbColor rgb="FF44546A"/>
+      <rgbColor rgb="FF3465A4"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -703,7 +675,7 @@
       <rgbColor rgb="FF385724"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF44546A"/>
       <rgbColor rgb="FF404040"/>
     </indexedColors>
   </colors>
@@ -718,14 +690,14 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="84.77"/>
@@ -980,7 +952,7 @@
       <c r="A13" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -994,7 +966,7 @@
       <c r="I13" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="22" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1031,7 +1003,7 @@
       <c r="E15" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="22"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
       <c r="J15" s="19" t="s">
@@ -1128,22 +1100,22 @@
       <c r="E20" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="23"/>
-      <c r="H20" s="24" t="s">
+      <c r="G20" s="24"/>
+      <c r="H20" s="25" t="s">
         <v>47</v>
       </c>
       <c r="J20" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="22" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -1154,18 +1126,18 @@
       <c r="F21" s="13"/>
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
-      <c r="J21" s="25" t="s">
+      <c r="J21" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="K21" s="26" t="s">
+      <c r="K21" s="22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="22" t="s">
         <v>51</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -1175,13 +1147,16 @@
       <c r="E22" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="23" t="s">
         <v>53</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
-      <c r="J22" s="17" t="s">
+      <c r="J22" s="22" t="s">
         <v>33</v>
+      </c>
+      <c r="K22" s="22" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,7 +1184,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9"/>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="26" t="s">
         <v>57</v>
       </c>
       <c r="C24" s="11"/>
@@ -1224,7 +1199,7 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9"/>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C25" s="11"/>
@@ -1298,7 +1273,7 @@
       <c r="D28" s="11"/>
       <c r="E28" s="20"/>
       <c r="F28" s="21"/>
-      <c r="G28" s="28" t="s">
+      <c r="G28" s="27" t="s">
         <v>67</v>
       </c>
       <c r="H28" s="15"/>
@@ -1380,7 +1355,7 @@
       <c r="A32" s="9" t="n">
         <v>25</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="28" t="s">
         <v>77</v>
       </c>
       <c r="C32" s="11" t="s">
@@ -1404,7 +1379,7 @@
       <c r="A33" s="9" t="n">
         <v>26</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="29" t="s">
         <v>81</v>
       </c>
       <c r="C33" s="11" t="s">
@@ -1426,7 +1401,7 @@
       <c r="A34" s="9" t="n">
         <v>27</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="30" t="s">
         <v>83</v>
       </c>
       <c r="C34" s="11" t="s">
@@ -1447,7 +1422,7 @@
       <c r="A35" s="9" t="n">
         <v>28</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="30" t="s">
         <v>85</v>
       </c>
       <c r="C35" s="11" t="s">
@@ -1510,7 +1485,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.22"/>
   </cols>

</xml_diff>